<commit_message>
Added pretty print to json file
</commit_message>
<xml_diff>
--- a/Cleaned Survey Results/surveydata.xlsx
+++ b/Cleaned Survey Results/surveydata.xlsx
@@ -1479,7 +1479,7 @@
         <v>4</v>
       </c>
       <c r="W2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X2">
         <v>2</v>
@@ -1631,7 +1631,7 @@
         <v>2</v>
       </c>
       <c r="W3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X3">
         <v>2</v>
@@ -1777,7 +1777,7 @@
         <v>3</v>
       </c>
       <c r="W4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X4">
         <v>1</v>
@@ -1926,7 +1926,7 @@
         <v>3</v>
       </c>
       <c r="W5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X5">
         <v>2</v>
@@ -2078,7 +2078,7 @@
         <v>2</v>
       </c>
       <c r="W6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -2224,7 +2224,7 @@
         <v>3</v>
       </c>
       <c r="W7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X7">
         <v>1</v>
@@ -2370,7 +2370,7 @@
         <v>4</v>
       </c>
       <c r="W8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X8">
         <v>1</v>
@@ -2525,7 +2525,7 @@
         <v>3</v>
       </c>
       <c r="W9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X9">
         <v>1</v>
@@ -2677,7 +2677,7 @@
         <v>5</v>
       </c>
       <c r="W10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X10">
         <v>3</v>
@@ -2823,7 +2823,7 @@
         <v>4</v>
       </c>
       <c r="W11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X11">
         <v>4</v>
@@ -2969,7 +2969,7 @@
         <v>3</v>
       </c>
       <c r="W12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X12">
         <v>2</v>
@@ -3115,7 +3115,7 @@
         <v>3</v>
       </c>
       <c r="W13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X13">
         <v>1</v>
@@ -3258,7 +3258,7 @@
         <v>3</v>
       </c>
       <c r="W14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X14">
         <v>5</v>
@@ -3404,7 +3404,7 @@
         <v>3</v>
       </c>
       <c r="W15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X15">
         <v>2</v>
@@ -3553,7 +3553,7 @@
         <v>2</v>
       </c>
       <c r="W16">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X16">
         <v>1</v>
@@ -3696,7 +3696,7 @@
         <v>1</v>
       </c>
       <c r="W17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X17">
         <v>3</v>
@@ -3845,7 +3845,7 @@
         <v>4</v>
       </c>
       <c r="W18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X18">
         <v>4</v>
@@ -3994,7 +3994,7 @@
         <v>2</v>
       </c>
       <c r="W19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X19">
         <v>4</v>
@@ -4140,7 +4140,7 @@
         <v>3</v>
       </c>
       <c r="W20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X20">
         <v>3</v>
@@ -4286,7 +4286,7 @@
         <v>1</v>
       </c>
       <c r="W21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X21">
         <v>1</v>
@@ -4435,7 +4435,7 @@
         <v>4</v>
       </c>
       <c r="W22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X22">
         <v>1</v>
@@ -4584,7 +4584,7 @@
         <v>4</v>
       </c>
       <c r="W23">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X23">
         <v>3</v>
@@ -4882,7 +4882,7 @@
         <v>2</v>
       </c>
       <c r="W25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X25">
         <v>3</v>
@@ -5028,7 +5028,7 @@
         <v>4</v>
       </c>
       <c r="W26">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X26">
         <v>4</v>
@@ -5174,7 +5174,7 @@
         <v>4</v>
       </c>
       <c r="W27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X27">
         <v>4</v>
@@ -5311,7 +5311,7 @@
         <v>5</v>
       </c>
       <c r="W28">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X28">
         <v>3</v>
@@ -5451,7 +5451,7 @@
         <v>4</v>
       </c>
       <c r="W29">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X29">
         <v>1</v>
@@ -5513,7 +5513,7 @@
       <c r="AQ29" t="b">
         <v>1</v>
       </c>
-      <c r="AR29" t="b">
+      <c r="AR29">
         <v>0</v>
       </c>
       <c r="AS29" t="b">
@@ -5606,7 +5606,7 @@
         <v>4</v>
       </c>
       <c r="W30">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="X30">
         <v>1</v>
@@ -5668,7 +5668,7 @@
       <c r="AQ30" t="b">
         <v>0</v>
       </c>
-      <c r="AR30" t="b">
+      <c r="AR30">
         <v>1</v>
       </c>
       <c r="AS30" t="b">
@@ -5770,7 +5770,7 @@
         <v>2</v>
       </c>
       <c r="W31">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="X31">
         <v>3</v>
@@ -5832,7 +5832,7 @@
       <c r="AQ31" t="b">
         <v>0</v>
       </c>
-      <c r="AR31" t="b">
+      <c r="AR31">
         <v>0</v>
       </c>
       <c r="AS31" t="b">
@@ -5931,7 +5931,7 @@
         <v>4</v>
       </c>
       <c r="W32">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X32">
         <v>4</v>
@@ -5990,7 +5990,7 @@
       <c r="AQ32" t="b">
         <v>0</v>
       </c>
-      <c r="AR32" t="b">
+      <c r="AR32">
         <v>0</v>
       </c>
       <c r="AS32" t="b">
@@ -6089,7 +6089,7 @@
         <v>2</v>
       </c>
       <c r="W33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X33">
         <v>2</v>
@@ -6148,7 +6148,7 @@
       <c r="AQ33" t="b">
         <v>0</v>
       </c>
-      <c r="AR33" t="b">
+      <c r="AR33">
         <v>0</v>
       </c>
       <c r="AS33" t="b">
@@ -6244,7 +6244,7 @@
         <v>3</v>
       </c>
       <c r="W34">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X34">
         <v>3</v>
@@ -6306,7 +6306,7 @@
       <c r="AQ34" t="b">
         <v>0</v>
       </c>
-      <c r="AR34" t="b">
+      <c r="AR34">
         <v>0</v>
       </c>
       <c r="AS34" t="b">
@@ -6405,7 +6405,7 @@
         <v>2</v>
       </c>
       <c r="W35">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="X35">
         <v>2</v>
@@ -6467,7 +6467,7 @@
       <c r="AQ35" t="b">
         <v>0</v>
       </c>
-      <c r="AR35" t="b">
+      <c r="AR35">
         <v>0</v>
       </c>
       <c r="AS35" t="b">
@@ -6557,7 +6557,7 @@
         <v>4</v>
       </c>
       <c r="W36">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="X36">
         <v>1</v>
@@ -6619,7 +6619,7 @@
       <c r="AQ36" t="b">
         <v>0</v>
       </c>
-      <c r="AR36" t="b">
+      <c r="AR36">
         <v>0</v>
       </c>
       <c r="AS36" t="b">
@@ -6715,7 +6715,7 @@
         <v>3</v>
       </c>
       <c r="W37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X37">
         <v>3</v>
@@ -6777,7 +6777,7 @@
       <c r="AQ37" t="b">
         <v>0</v>
       </c>
-      <c r="AR37" t="b">
+      <c r="AR37">
         <v>1</v>
       </c>
       <c r="AS37" t="b">
@@ -6938,7 +6938,7 @@
       <c r="AQ38" t="b">
         <v>0</v>
       </c>
-      <c r="AR38" t="b">
+      <c r="AR38">
         <v>0</v>
       </c>
       <c r="AS38" t="b">
@@ -7102,7 +7102,7 @@
       <c r="AQ39" t="b">
         <v>0</v>
       </c>
-      <c r="AR39" t="b">
+      <c r="AR39">
         <v>1</v>
       </c>
       <c r="AS39" t="b">
@@ -7254,7 +7254,7 @@
       <c r="AQ40" t="b">
         <v>0</v>
       </c>
-      <c r="AR40" t="b">
+      <c r="AR40">
         <v>0</v>
       </c>
       <c r="AS40" t="b">
@@ -7412,7 +7412,7 @@
       <c r="AQ41" t="b">
         <v>0</v>
       </c>
-      <c r="AR41" t="b">
+      <c r="AR41">
         <v>0</v>
       </c>
       <c r="AS41" t="b">
@@ -7564,7 +7564,7 @@
       <c r="AQ42" t="b">
         <v>1</v>
       </c>
-      <c r="AR42" t="b">
+      <c r="AR42">
         <v>0</v>
       </c>
       <c r="AS42" t="b">
@@ -7722,7 +7722,7 @@
       <c r="AQ43" t="b">
         <v>1</v>
       </c>
-      <c r="AR43" t="b">
+      <c r="AR43">
         <v>0</v>
       </c>
       <c r="AS43" t="b">
@@ -7871,7 +7871,7 @@
       <c r="AQ44" t="b">
         <v>0</v>
       </c>
-      <c r="AR44" t="b">
+      <c r="AR44">
         <v>0</v>
       </c>
       <c r="AS44" t="b">
@@ -8026,7 +8026,7 @@
       <c r="AQ45" t="b">
         <v>0</v>
       </c>
-      <c r="AR45" t="b">
+      <c r="AR45">
         <v>1</v>
       </c>
       <c r="AS45" t="b">
@@ -8178,7 +8178,7 @@
       <c r="AQ46" t="b">
         <v>0</v>
       </c>
-      <c r="AR46" t="b">
+      <c r="AR46">
         <v>0</v>
       </c>
       <c r="AS46" t="b">
@@ -8339,7 +8339,7 @@
       <c r="AQ47" t="b">
         <v>1</v>
       </c>
-      <c r="AR47" t="b">
+      <c r="AR47">
         <v>0</v>
       </c>
       <c r="AS47" t="b">
@@ -8497,7 +8497,7 @@
       <c r="AQ48" t="b">
         <v>0</v>
       </c>
-      <c r="AR48" t="b">
+      <c r="AR48">
         <v>1</v>
       </c>
       <c r="AS48" t="b">
@@ -8658,7 +8658,7 @@
       <c r="AQ49" t="b">
         <v>0</v>
       </c>
-      <c r="AR49" t="b">
+      <c r="AR49">
         <v>1</v>
       </c>
       <c r="AS49" t="b">
@@ -8816,7 +8816,7 @@
       <c r="AQ50" t="b">
         <v>1</v>
       </c>
-      <c r="AR50" t="b">
+      <c r="AR50">
         <v>0</v>
       </c>
       <c r="AS50" t="b">

</xml_diff>